<commit_message>
Updated with new version added Exact match usecase
</commit_message>
<xml_diff>
--- a/src/test/resources/css/customer-self-service.xlsx
+++ b/src/test/resources/css/customer-self-service.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Elan\virtualan-software-ws\august-release\microservices-lowcode-testautomation\src\test\resources\css\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5453BDAB-EB85-4335-AFB1-9CC2D67166B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1770D47-FFD3-4367-A7B4-54C74B9E9F7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{7CA6F974-39B2-4E5F-BC2D-5AC16F3752B6}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="71">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -298,9 +298,6 @@
     <t>success=c~LEN("[firstname]")=3</t>
   </si>
   <si>
-    <t>customer</t>
-  </si>
-  <si>
     <t>http://microservices.virtualandemo.com:8090/customers</t>
   </si>
   <si>
@@ -310,7 +307,35 @@
     <t>Read Customer infos</t>
   </si>
   <si>
-    <t>ReadCustomers</t>
+    <t>Read Customer infos - Exact-Order-Match</t>
+  </si>
+  <si>
+    <t>ReadCustomers-EOM</t>
+  </si>
+  <si>
+    <t>jsonpath=customers;match=exact-order-match
+customerId,firstname,lastname,postalCode,streetAddress
+bunlo9vk5f,Ado,Kinnett,6500,2 Autumn Leaf Lane</t>
+  </si>
+  <si>
+    <t>https://live.virtualandemo.com/api/persons/bgates</t>
+  </si>
+  <si>
+    <t>ReadCustomers-Simple</t>
+  </si>
+  <si>
+    <t>dateOfBirth,firstName,lastName,lastTimeOnline,spokenLanguages/additionalProp1:additionalProp2:additionalProp3,username
+1955-10-28,Bill,Gates,2020-08-30T20:28:36.267Z,Tamil:English:Spanish,bgates</t>
+  </si>
+  <si>
+    <t>match=exact-order-match
+dateOfBirth,lastName,firstName,lastTimeOnline,spokenLanguages/additionalProp1:additionalProp3:additionalProp2
+1955-10-28,Gates,Bill,2020-08-30T20:28:36.267Z,Tamil:Spanish:English</t>
+  </si>
+  <si>
+    <t>match=exact-match
+dateOfBirth,firstName,lastName,lastTimeOnline,spokenLanguages/additionalProp1:additionalProp3:additionalProp2,username
+1955-10-28,Bill,Gates,2020-08-30T20:28:36.267Z,Tamil:Spanish:English,bgates</t>
   </si>
 </sst>
 </file>
@@ -1098,8 +1123,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D2DC3DC4-786B-455B-AC31-440CB4CE2386}" name="Table13" displayName="Table13" ref="A1:O8" totalsRowShown="0" headerRowDxfId="36" headerRowBorderDxfId="35" tableBorderDxfId="34" totalsRowBorderDxfId="33">
-  <autoFilter ref="A1:O8" xr:uid="{9ED465CD-F594-48A9-8196-5FC7750F944C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D2DC3DC4-786B-455B-AC31-440CB4CE2386}" name="Table13" displayName="Table13" ref="A1:O11" totalsRowShown="0" headerRowDxfId="36" headerRowBorderDxfId="35" tableBorderDxfId="34" totalsRowBorderDxfId="33">
+  <autoFilter ref="A1:O11" xr:uid="{9ED465CD-F594-48A9-8196-5FC7750F944C}"/>
   <tableColumns count="15">
     <tableColumn id="1" xr3:uid="{2529773C-869E-4BF0-BA40-3C63A1B9C82E}" name="TestCaseName" dataDxfId="32"/>
     <tableColumn id="2" xr3:uid="{38B39313-4971-4AB8-90FF-17FEEBD272E2}" name="Type" dataDxfId="31"/>
@@ -1441,10 +1466,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B87A57E5-F5BD-4861-8936-9E28488C0E70}">
-  <dimension ref="A1:O8"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1452,7 +1477,7 @@
     <col min="1" max="1" width="30.68359375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.41796875" customWidth="1"/>
     <col min="3" max="3" width="12.41796875" customWidth="1"/>
-    <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.7890625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="81" customWidth="1"/>
     <col min="6" max="6" width="8.83984375" customWidth="1"/>
     <col min="7" max="7" width="16.15625" customWidth="1"/>
@@ -1461,7 +1486,7 @@
     <col min="10" max="10" width="54.578125" customWidth="1"/>
     <col min="11" max="11" width="58.89453125" customWidth="1"/>
     <col min="12" max="12" width="25.26171875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.68359375" customWidth="1"/>
+    <col min="13" max="13" width="111.83984375" customWidth="1"/>
     <col min="14" max="14" width="25.47265625" customWidth="1"/>
     <col min="15" max="15" width="14.83984375" customWidth="1"/>
   </cols>
@@ -1593,21 +1618,19 @@
       </c>
       <c r="O3" s="9"/>
     </row>
-    <row r="4" spans="1:15" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:15" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="5" t="s">
         <v>64</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>60</v>
-      </c>
+      <c r="C4" s="6"/>
       <c r="D4" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>19</v>
@@ -1620,29 +1643,27 @@
       </c>
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
-      <c r="K4" s="15" t="s">
-        <v>62</v>
-      </c>
+      <c r="K4" s="15"/>
       <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
+      <c r="M4" s="11" t="s">
+        <v>70</v>
+      </c>
       <c r="N4" s="6"/>
       <c r="O4" s="6"/>
     </row>
-    <row r="5" spans="1:15" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:15" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="5" t="s">
-        <v>22</v>
+        <v>64</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>22</v>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>23</v>
+        <v>66</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>19</v>
@@ -1653,40 +1674,32 @@
       <c r="H5" s="6">
         <v>200</v>
       </c>
-      <c r="I5" s="6" t="s">
-        <v>27</v>
-      </c>
+      <c r="I5" s="6"/>
       <c r="J5" s="6"/>
-      <c r="K5" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="L5" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="M5" s="9"/>
-      <c r="N5" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="O5" s="9"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
     </row>
-    <row r="6" spans="1:15" ht="374.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:15" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="5" t="s">
-        <v>32</v>
+        <v>67</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>32</v>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6" t="s">
+        <v>62</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>31</v>
+        <v>66</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>12</v>
@@ -1694,25 +1707,19 @@
       <c r="H6" s="6">
         <v>200</v>
       </c>
-      <c r="I6" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="J6" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="K6" s="8"/>
-      <c r="L6" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="M6" s="9"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9" t="s">
-        <v>56</v>
-      </c>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
     </row>
-    <row r="7" spans="1:15" ht="172.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:15" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="5" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>8</v>
@@ -1720,14 +1727,14 @@
       <c r="C7" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D7" s="5" t="s">
-        <v>40</v>
+      <c r="D7" s="6" t="s">
+        <v>63</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>33</v>
+        <v>60</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>12</v>
@@ -1735,23 +1742,21 @@
       <c r="H7" s="6">
         <v>200</v>
       </c>
-      <c r="I7" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="J7" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="K7" s="8" t="s">
-        <v>34</v>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="15" t="s">
+        <v>61</v>
       </c>
       <c r="L7" s="6"/>
-      <c r="M7" s="9"/>
-      <c r="N7" s="9"/>
-      <c r="O7" s="9"/>
+      <c r="M7" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
     </row>
-    <row r="8" spans="1:15" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:15" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="5" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>8</v>
@@ -1760,13 +1765,13 @@
         <v>9</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>36</v>
+        <v>22</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>35</v>
+        <v>19</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>12</v>
@@ -1777,34 +1782,156 @@
       <c r="I8" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="J8" s="11" t="s">
+      <c r="J8" s="6"/>
+      <c r="K8" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="L8" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="M8" s="9"/>
+      <c r="N8" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="O8" s="9"/>
+    </row>
+    <row r="9" spans="1:15" ht="374.4" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="6">
+        <v>200</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="J9" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="K9" s="8"/>
+      <c r="L9" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="M9" s="9"/>
+      <c r="N9" s="9"/>
+      <c r="O9" s="9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="172.8" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G10" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="6">
+        <v>200</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="J10" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="L10" s="6"/>
+      <c r="M10" s="9"/>
+      <c r="N10" s="9"/>
+      <c r="O10" s="9"/>
+    </row>
+    <row r="11" spans="1:15" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="6">
+        <v>200</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="J11" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="K8" s="8" t="s">
+      <c r="K11" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="L8" s="6"/>
-      <c r="M8" s="13" t="s">
+      <c r="L11" s="6"/>
+      <c r="M11" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="N8" s="9"/>
-      <c r="O8" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{D386C033-F1AE-4CEA-BD21-276011470BBA}"/>
     <hyperlink ref="E3" r:id="rId2" xr:uid="{B6FF64BC-A07C-4862-8BCF-29E7D9C8AED9}"/>
     <hyperlink ref="K3" r:id="rId3" display="email=admin@example.com" xr:uid="{6578FDF2-846E-4A5F-AFC5-42766B4B0470}"/>
-    <hyperlink ref="E5" r:id="rId4" xr:uid="{18970103-3D15-4C34-A217-1990C9B8F8E3}"/>
-    <hyperlink ref="K2" r:id="rId5" display="email=admin@example.com" xr:uid="{FA7D36A9-A6DA-4DA4-881D-45A3E3E86790}"/>
-    <hyperlink ref="E6" r:id="rId6" xr:uid="{D708BF3F-71AB-4960-BC00-99A558F06D6B}"/>
-    <hyperlink ref="E7" r:id="rId7" xr:uid="{3289CF67-1AB2-4462-B560-3335CDDCCDBD}"/>
-    <hyperlink ref="E8" r:id="rId8" xr:uid="{87B049EE-CC57-404F-9C99-F6D58B93183E}"/>
+    <hyperlink ref="K2" r:id="rId4" display="email=admin@example.com" xr:uid="{FA7D36A9-A6DA-4DA4-881D-45A3E3E86790}"/>
+    <hyperlink ref="E10" r:id="rId5" xr:uid="{3289CF67-1AB2-4462-B560-3335CDDCCDBD}"/>
+    <hyperlink ref="E11" r:id="rId6" xr:uid="{87B049EE-CC57-404F-9C99-F6D58B93183E}"/>
+    <hyperlink ref="E7" r:id="rId7" xr:uid="{63206C17-F1C8-48C0-95B7-F0A0AD92D0FC}"/>
+    <hyperlink ref="E9" r:id="rId8" xr:uid="{D708BF3F-71AB-4960-BC00-99A558F06D6B}"/>
+    <hyperlink ref="E8" r:id="rId9" xr:uid="{18970103-3D15-4C34-A217-1990C9B8F8E3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId9"/>
+  <pageSetup orientation="portrait" r:id="rId10"/>
   <tableParts count="1">
-    <tablePart r:id="rId10"/>
+    <tablePart r:id="rId11"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Examples added as separate sheet
</commit_message>
<xml_diff>
--- a/src/test/resources/css/customer-self-service.xlsx
+++ b/src/test/resources/css/customer-self-service.xlsx
@@ -5,16 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Elan\virtualan-software-ws\august-release\microservices-lowcode-testautomation\src\test\resources\css\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\virtualan-software-delivery\September-release\microservices-lowcode-testautomation\src\test\resources\css\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1770D47-FFD3-4367-A7B4-54C74B9E9F7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED2E47B-65F6-45BD-97DA-728B53A8CE5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{7CA6F974-39B2-4E5F-BC2D-5AC16F3752B6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{7CA6F974-39B2-4E5F-BC2D-5AC16F3752B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer Self Service-Accept" sheetId="2" r:id="rId1"/>
     <sheet name="Customer Self-Service-Reject" sheetId="1" r:id="rId2"/>
+    <sheet name="Examples" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="74">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -304,9 +305,6 @@
     <t>customers.find { it.firstname \\=\\= 'Ado' }.postalCode=6500;customers.find { it.customerId \\=\\= 'bunlo9vk5f' }.firstname=Ado;customers.find { it.customerId \\=\\= 'f2m0v9b73c' }.email=blangman14@example.com;</t>
   </si>
   <si>
-    <t>Read Customer infos</t>
-  </si>
-  <si>
     <t>Read Customer infos - Exact-Order-Match</t>
   </si>
   <si>
@@ -336,6 +334,18 @@
     <t>match=exact-match
 dateOfBirth,firstName,lastName,lastTimeOnline,spokenLanguages/additionalProp1:additionalProp3:additionalProp2,username
 1955-10-28,Bill,Gates,2020-08-30T20:28:36.267Z,Tamil:Spanish:English,bgates</t>
+  </si>
+  <si>
+    <t>ReadCustomers</t>
+  </si>
+  <si>
+    <t>Read Customer infos - Example-case1</t>
+  </si>
+  <si>
+    <t>Read Customer infos - Example-case2</t>
+  </si>
+  <si>
+    <t>Read Customer infos - Example-case3</t>
   </si>
 </sst>
 </file>
@@ -1466,32 +1476,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B87A57E5-F5BD-4861-8936-9E28488C0E70}">
-  <dimension ref="A1:O11"/>
+  <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.68359375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.41796875" customWidth="1"/>
-    <col min="3" max="3" width="12.41796875" customWidth="1"/>
-    <col min="4" max="4" width="33.7890625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="33.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="81" customWidth="1"/>
-    <col min="6" max="6" width="8.83984375" customWidth="1"/>
-    <col min="7" max="7" width="16.15625" customWidth="1"/>
-    <col min="8" max="8" width="14.83984375" customWidth="1"/>
-    <col min="9" max="9" width="21.15625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="54.578125" customWidth="1"/>
-    <col min="11" max="11" width="58.89453125" customWidth="1"/>
-    <col min="12" max="12" width="25.26171875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="111.83984375" customWidth="1"/>
-    <col min="14" max="14" width="25.47265625" customWidth="1"/>
-    <col min="15" max="15" width="14.83984375" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" customWidth="1"/>
+    <col min="9" max="9" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="54.5703125" customWidth="1"/>
+    <col min="11" max="11" width="58.85546875" customWidth="1"/>
+    <col min="12" max="12" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="111.85546875" customWidth="1"/>
+    <col min="14" max="14" width="25.42578125" customWidth="1"/>
+    <col min="15" max="15" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1538,7 +1548,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>28</v>
       </c>
@@ -1577,7 +1587,7 @@
       <c r="N2" s="9"/>
       <c r="O2" s="9"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>21</v>
       </c>
@@ -1618,19 +1628,21 @@
       </c>
       <c r="O3" s="9"/>
     </row>
-    <row r="4" spans="1:15" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>64</v>
+        <v>22</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6" t="s">
-        <v>62</v>
+      <c r="C4" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>66</v>
+        <v>23</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>19</v>
@@ -1641,32 +1653,40 @@
       <c r="H4" s="6">
         <v>200</v>
       </c>
-      <c r="I4" s="6"/>
+      <c r="I4" s="6" t="s">
+        <v>27</v>
+      </c>
       <c r="J4" s="6"/>
-      <c r="K4" s="15"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
+      <c r="K4" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="L4" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="M4" s="9"/>
+      <c r="N4" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="O4" s="9"/>
     </row>
-    <row r="5" spans="1:15" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:15" ht="390" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>64</v>
+        <v>32</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6" t="s">
-        <v>62</v>
+      <c r="C5" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>32</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>66</v>
+        <v>31</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>12</v>
@@ -1674,32 +1694,40 @@
       <c r="H5" s="6">
         <v>200</v>
       </c>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="11" t="s">
-        <v>69</v>
-      </c>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
+      <c r="I5" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="K5" s="8"/>
+      <c r="L5" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="M5" s="9"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="9" t="s">
+        <v>56</v>
+      </c>
     </row>
-    <row r="6" spans="1:15" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:15" ht="180" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>67</v>
+        <v>40</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6" t="s">
-        <v>62</v>
+      <c r="C6" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>40</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>66</v>
+        <v>33</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>12</v>
@@ -1707,34 +1735,38 @@
       <c r="H6" s="6">
         <v>200</v>
       </c>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="15"/>
+      <c r="I6" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="K6" s="8" t="s">
+        <v>34</v>
+      </c>
       <c r="L6" s="6"/>
-      <c r="M6" s="11" t="s">
-        <v>68</v>
-      </c>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
+      <c r="M6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
     </row>
-    <row r="7" spans="1:15" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>64</v>
+        <v>36</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>63</v>
+        <v>9</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>19</v>
+        <v>35</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>12</v>
@@ -1742,179 +1774,21 @@
       <c r="H7" s="6">
         <v>200</v>
       </c>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
-      <c r="K7" s="15" t="s">
-        <v>61</v>
+      <c r="I7" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="K7" s="8" t="s">
+        <v>34</v>
       </c>
       <c r="L7" s="6"/>
-      <c r="M7" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
-    </row>
-    <row r="8" spans="1:15" ht="72" x14ac:dyDescent="0.55000000000000004">
-      <c r="A8" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E8" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="6">
-        <v>200</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="J8" s="6"/>
-      <c r="K8" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="L8" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="M8" s="9"/>
-      <c r="N8" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="O8" s="9"/>
-    </row>
-    <row r="9" spans="1:15" ht="374.4" x14ac:dyDescent="0.55000000000000004">
-      <c r="A9" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="B9" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H9" s="6">
-        <v>200</v>
-      </c>
-      <c r="I9" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="J9" s="11" t="s">
-        <v>57</v>
-      </c>
-      <c r="K9" s="8"/>
-      <c r="L9" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="M9" s="9"/>
-      <c r="N9" s="9"/>
-      <c r="O9" s="9" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" ht="172.8" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B10" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C10" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H10" s="6">
-        <v>200</v>
-      </c>
-      <c r="I10" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="J10" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="K10" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="L10" s="6"/>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="9"/>
-    </row>
-    <row r="11" spans="1:15" ht="43.2" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C11" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G11" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="H11" s="6">
-        <v>200</v>
-      </c>
-      <c r="I11" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="J11" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="K11" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="L11" s="6"/>
-      <c r="M11" s="13" t="s">
+      <c r="M7" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="N11" s="9"/>
-      <c r="O11" s="9"/>
+      <c r="N7" s="9"/>
+      <c r="O7" s="9"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1922,16 +1796,15 @@
     <hyperlink ref="E3" r:id="rId2" xr:uid="{B6FF64BC-A07C-4862-8BCF-29E7D9C8AED9}"/>
     <hyperlink ref="K3" r:id="rId3" display="email=admin@example.com" xr:uid="{6578FDF2-846E-4A5F-AFC5-42766B4B0470}"/>
     <hyperlink ref="K2" r:id="rId4" display="email=admin@example.com" xr:uid="{FA7D36A9-A6DA-4DA4-881D-45A3E3E86790}"/>
-    <hyperlink ref="E10" r:id="rId5" xr:uid="{3289CF67-1AB2-4462-B560-3335CDDCCDBD}"/>
-    <hyperlink ref="E11" r:id="rId6" xr:uid="{87B049EE-CC57-404F-9C99-F6D58B93183E}"/>
-    <hyperlink ref="E7" r:id="rId7" xr:uid="{63206C17-F1C8-48C0-95B7-F0A0AD92D0FC}"/>
-    <hyperlink ref="E9" r:id="rId8" xr:uid="{D708BF3F-71AB-4960-BC00-99A558F06D6B}"/>
-    <hyperlink ref="E8" r:id="rId9" xr:uid="{18970103-3D15-4C34-A217-1990C9B8F8E3}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{3289CF67-1AB2-4462-B560-3335CDDCCDBD}"/>
+    <hyperlink ref="E7" r:id="rId6" xr:uid="{87B049EE-CC57-404F-9C99-F6D58B93183E}"/>
+    <hyperlink ref="E5" r:id="rId7" xr:uid="{D708BF3F-71AB-4960-BC00-99A558F06D6B}"/>
+    <hyperlink ref="E4" r:id="rId8" xr:uid="{18970103-3D15-4C34-A217-1990C9B8F8E3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId10"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
   <tableParts count="1">
-    <tablePart r:id="rId11"/>
+    <tablePart r:id="rId10"/>
   </tableParts>
 </worksheet>
 </file>
@@ -1944,24 +1817,24 @@
       <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.68359375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.41796875" customWidth="1"/>
-    <col min="3" max="3" width="12.41796875" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
     <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="80.15625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.83984375" customWidth="1"/>
-    <col min="7" max="7" width="16.15625" customWidth="1"/>
-    <col min="8" max="8" width="14.83984375" customWidth="1"/>
-    <col min="9" max="9" width="21.15625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="54.578125" customWidth="1"/>
+    <col min="5" max="5" width="80.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" customWidth="1"/>
+    <col min="9" max="9" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="54.5703125" customWidth="1"/>
     <col min="11" max="11" width="27" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.26171875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24.62890625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2005,7 +1878,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>28</v>
       </c>
@@ -2043,7 +1916,7 @@
       <c r="M2" s="9"/>
       <c r="N2" s="9"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>21</v>
       </c>
@@ -2081,7 +1954,7 @@
       <c r="M3" s="9"/>
       <c r="N3" s="9"/>
     </row>
-    <row r="4" spans="1:14" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>22</v>
       </c>
@@ -2119,7 +1992,7 @@
       <c r="M4" s="9"/>
       <c r="N4" s="9"/>
     </row>
-    <row r="5" spans="1:14" ht="374.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:14" ht="390" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>47</v>
       </c>
@@ -2157,7 +2030,7 @@
       <c r="M5" s="9"/>
       <c r="N5" s="9"/>
     </row>
-    <row r="6" spans="1:14" ht="172.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:14" ht="180" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>46</v>
       </c>
@@ -2195,7 +2068,7 @@
       <c r="M6" s="9"/>
       <c r="N6" s="9"/>
     </row>
-    <row r="7" spans="1:14" ht="158.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:14" ht="195" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>41</v>
       </c>
@@ -2252,4 +2125,181 @@
     <tablePart r:id="rId10"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50E57E3D-0C14-46A6-9520-2A3B86BE3763}">
+  <dimension ref="A1:J5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="53" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="55.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="65.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="J1" s="12" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="E2" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="6">
+        <v>200</v>
+      </c>
+      <c r="I2" s="15"/>
+      <c r="J2" s="11" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" s="6">
+        <v>200</v>
+      </c>
+      <c r="I3" s="15"/>
+      <c r="J3" s="11" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4" s="6">
+        <v>200</v>
+      </c>
+      <c r="I4" s="15"/>
+      <c r="J4" s="11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H5" s="6">
+        <v>200</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E5" r:id="rId1" xr:uid="{63206C17-F1C8-48C0-95B7-F0A0AD92D0FC}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated with Few more examples
</commit_message>
<xml_diff>
--- a/src/test/resources/css/customer-self-service.xlsx
+++ b/src/test/resources/css/customer-self-service.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\virtualan-software-delivery\September-release\microservices-lowcode-testautomation\src\test\resources\css\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Elan\virtualan-software-ws\september-release\microservices-lowcode-testautomation\src\test\resources\css\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AED2E47B-65F6-45BD-97DA-728B53A8CE5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C7BC13D-7312-4BF0-A8FF-5421279D4424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{7CA6F974-39B2-4E5F-BC2D-5AC16F3752B6}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{7CA6F974-39B2-4E5F-BC2D-5AC16F3752B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer Self Service-Accept" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="80">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -346,6 +346,27 @@
   </si>
   <si>
     <t>Read Customer infos - Example-case3</t>
+  </si>
+  <si>
+    <t>{
+  "birthday" : "1918-10-24",
+  "postalCode" : "60563"
+}</t>
+  </si>
+  <si>
+    <t>https://live.virtualandemo.com/api/riskfactor/compute</t>
+  </si>
+  <si>
+    <t>RiskFactor-DirtectResponse</t>
+  </si>
+  <si>
+    <t>riskFactor=.</t>
+  </si>
+  <si>
+    <t>ResponseContent</t>
+  </si>
+  <si>
+    <t>success=c~[riskFactor]=65</t>
   </si>
 </sst>
 </file>
@@ -397,7 +418,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -499,12 +520,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -529,6 +559,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1478,30 +1514,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B87A57E5-F5BD-4861-8936-9E28488C0E70}">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="N4" sqref="N4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" customWidth="1"/>
-    <col min="4" max="4" width="33.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.68359375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.41796875" customWidth="1"/>
+    <col min="3" max="3" width="12.41796875" customWidth="1"/>
+    <col min="4" max="4" width="33.83984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="81" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" customWidth="1"/>
-    <col min="9" max="9" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="54.5703125" customWidth="1"/>
-    <col min="11" max="11" width="58.85546875" customWidth="1"/>
-    <col min="12" max="12" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="111.85546875" customWidth="1"/>
-    <col min="14" max="14" width="25.42578125" customWidth="1"/>
-    <col min="15" max="15" width="14.85546875" customWidth="1"/>
+    <col min="6" max="6" width="8.83984375" customWidth="1"/>
+    <col min="7" max="7" width="16.15625" customWidth="1"/>
+    <col min="8" max="8" width="14.83984375" customWidth="1"/>
+    <col min="9" max="9" width="21.15625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="54.578125" customWidth="1"/>
+    <col min="11" max="11" width="58.83984375" customWidth="1"/>
+    <col min="12" max="12" width="25.26171875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="111.83984375" customWidth="1"/>
+    <col min="14" max="14" width="25.41796875" customWidth="1"/>
+    <col min="15" max="15" width="14.83984375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1548,7 +1584,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="5" t="s">
         <v>28</v>
       </c>
@@ -1587,7 +1623,7 @@
       <c r="N2" s="9"/>
       <c r="O2" s="9"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="5" t="s">
         <v>21</v>
       </c>
@@ -1628,7 +1664,7 @@
       </c>
       <c r="O3" s="9"/>
     </row>
-    <row r="4" spans="1:15" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="5" t="s">
         <v>22</v>
       </c>
@@ -1669,7 +1705,7 @@
       </c>
       <c r="O4" s="9"/>
     </row>
-    <row r="5" spans="1:15" ht="390" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" ht="374.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="5" t="s">
         <v>32</v>
       </c>
@@ -1710,7 +1746,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="180" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="5" t="s">
         <v>40</v>
       </c>
@@ -1749,7 +1785,7 @@
       <c r="N6" s="9"/>
       <c r="O6" s="9"/>
     </row>
-    <row r="7" spans="1:15" ht="45" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="5" t="s">
         <v>36</v>
       </c>
@@ -1813,28 +1849,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{558B51E2-E984-41DF-9C0A-F557E24A35FA}">
   <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView topLeftCell="K3" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="1" max="1" width="30.68359375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.41796875" customWidth="1"/>
+    <col min="3" max="3" width="12.41796875" customWidth="1"/>
     <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="80.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" customWidth="1"/>
-    <col min="7" max="7" width="16.140625" customWidth="1"/>
-    <col min="8" max="8" width="14.85546875" customWidth="1"/>
-    <col min="9" max="9" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="54.5703125" customWidth="1"/>
+    <col min="5" max="5" width="80.15625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.83984375" customWidth="1"/>
+    <col min="7" max="7" width="16.15625" customWidth="1"/>
+    <col min="8" max="8" width="14.83984375" customWidth="1"/>
+    <col min="9" max="9" width="21.15625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="54.578125" customWidth="1"/>
     <col min="11" max="11" width="27" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.26171875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1878,7 +1914,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="5" t="s">
         <v>28</v>
       </c>
@@ -1916,7 +1952,7 @@
       <c r="M2" s="9"/>
       <c r="N2" s="9"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="5" t="s">
         <v>21</v>
       </c>
@@ -1954,7 +1990,7 @@
       <c r="M3" s="9"/>
       <c r="N3" s="9"/>
     </row>
-    <row r="4" spans="1:14" ht="75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="72" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="5" t="s">
         <v>22</v>
       </c>
@@ -1992,7 +2028,7 @@
       <c r="M4" s="9"/>
       <c r="N4" s="9"/>
     </row>
-    <row r="5" spans="1:14" ht="390" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="374.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="5" t="s">
         <v>47</v>
       </c>
@@ -2030,7 +2066,7 @@
       <c r="M5" s="9"/>
       <c r="N5" s="9"/>
     </row>
-    <row r="6" spans="1:14" ht="180" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="172.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="5" t="s">
         <v>46</v>
       </c>
@@ -2068,7 +2104,7 @@
       <c r="M6" s="9"/>
       <c r="N6" s="9"/>
     </row>
-    <row r="7" spans="1:14" ht="195" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="158.4" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="5" t="s">
         <v>41</v>
       </c>
@@ -2129,26 +2165,29 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50E57E3D-0C14-46A6-9520-2A3B86BE3763}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:N6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.15625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.26171875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.41796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="53" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="55.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="65.42578125" customWidth="1"/>
+    <col min="6" max="6" width="6.68359375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.26171875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="34.47265625" customWidth="1"/>
+    <col min="11" max="11" width="55.41796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="65.41796875" customWidth="1"/>
+    <col min="13" max="13" width="20.578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="28.05078125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2173,14 +2212,26 @@
       <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="I1" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="K1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="J1" s="12" t="s">
+      <c r="L1" s="12" t="s">
         <v>48</v>
       </c>
+      <c r="M1" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="19" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="5" t="s">
         <v>70</v>
       </c>
@@ -2203,12 +2254,14 @@
       <c r="H2" s="6">
         <v>200</v>
       </c>
-      <c r="I2" s="15"/>
-      <c r="J2" s="11" t="s">
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="11" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="5" t="s">
         <v>63</v>
       </c>
@@ -2231,12 +2284,14 @@
       <c r="H3" s="6">
         <v>200</v>
       </c>
-      <c r="I3" s="15"/>
-      <c r="J3" s="11" t="s">
+      <c r="I3" s="17"/>
+      <c r="J3" s="17"/>
+      <c r="K3" s="15"/>
+      <c r="L3" s="11" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="5" t="s">
         <v>66</v>
       </c>
@@ -2259,12 +2314,14 @@
       <c r="H4" s="6">
         <v>200</v>
       </c>
-      <c r="I4" s="15"/>
-      <c r="J4" s="11" t="s">
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="15"/>
+      <c r="L4" s="11" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="60" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="5" t="s">
         <v>63</v>
       </c>
@@ -2289,16 +2346,56 @@
       <c r="H5" s="6">
         <v>200</v>
       </c>
-      <c r="I5" s="15" t="s">
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="J5" s="11" t="s">
+      <c r="L5" s="11" t="s">
         <v>64</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="H6" s="6">
+        <v>200</v>
+      </c>
+      <c r="I6" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="J6" s="18">
+        <v>65</v>
+      </c>
+      <c r="M6" t="s">
+        <v>77</v>
+      </c>
+      <c r="N6" t="s">
+        <v>79</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E5" r:id="rId1" xr:uid="{63206C17-F1C8-48C0-95B7-F0A0AD92D0FC}"/>
+    <hyperlink ref="E6" r:id="rId2" xr:uid="{222B9008-B6F1-43AD-AB02-552007F39E4F}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{4201C29B-B67D-48C2-92AE-011AA2CEB9F2}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated Jenkins and new release version
</commit_message>
<xml_diff>
--- a/src/test/resources/css/customer-self-service.xlsx
+++ b/src/test/resources/css/customer-self-service.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Elan\virtualan-software-ws\september-release\microservices-lowcode-testautomation\src\test\resources\css\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C7BC13D-7312-4BF0-A8FF-5421279D4424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E99519C9-8301-4A85-8F9D-BA7423C22F0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{7CA6F974-39B2-4E5F-BC2D-5AC16F3752B6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="83">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -367,6 +367,15 @@
   </si>
   <si>
     <t>success=c~[riskFactor]=65</t>
+  </si>
+  <si>
+    <t>Tags</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @examples</t>
+  </si>
+  <si>
+    <t>@examples</t>
   </si>
 </sst>
 </file>
@@ -2165,10 +2174,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50E57E3D-0C14-46A6-9520-2A3B86BE3763}">
-  <dimension ref="A1:N6"/>
+  <dimension ref="A1:O6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -2187,7 +2196,7 @@
     <col min="14" max="14" width="28.05078125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2230,8 +2239,11 @@
       <c r="N1" s="19" t="s">
         <v>53</v>
       </c>
+      <c r="O1" s="19" t="s">
+        <v>80</v>
+      </c>
     </row>
-    <row r="2" spans="1:14" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:15" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="5" t="s">
         <v>70</v>
       </c>
@@ -2260,8 +2272,11 @@
       <c r="L2" s="11" t="s">
         <v>69</v>
       </c>
+      <c r="O2" t="s">
+        <v>82</v>
+      </c>
     </row>
-    <row r="3" spans="1:14" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:15" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="5" t="s">
         <v>63</v>
       </c>
@@ -2290,8 +2305,11 @@
       <c r="L3" s="11" t="s">
         <v>68</v>
       </c>
+      <c r="O3" t="s">
+        <v>81</v>
+      </c>
     </row>
-    <row r="4" spans="1:14" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:15" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="5" t="s">
         <v>66</v>
       </c>
@@ -2320,8 +2338,11 @@
       <c r="L4" s="11" t="s">
         <v>67</v>
       </c>
+      <c r="O4" t="s">
+        <v>82</v>
+      </c>
     </row>
-    <row r="5" spans="1:14" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:15" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="5" t="s">
         <v>63</v>
       </c>
@@ -2354,8 +2375,11 @@
       <c r="L5" s="11" t="s">
         <v>64</v>
       </c>
+      <c r="O5" t="s">
+        <v>82</v>
+      </c>
     </row>
-    <row r="6" spans="1:14" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:15" ht="57.6" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="5" t="s">
         <v>76</v>
       </c>
@@ -2389,6 +2413,9 @@
       </c>
       <c r="N6" t="s">
         <v>79</v>
+      </c>
+      <c r="O6" t="s">
+        <v>82</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated with UTC timezone using Excel functions
</commit_message>
<xml_diff>
--- a/src/test/resources/css/customer-self-service.xlsx
+++ b/src/test/resources/css/customer-self-service.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Elan\virtualan-software-ws\september-release\microservices-lowcode-testautomation\src\test\resources\css\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\virtualan-software-delivery\September-release\microservices-lowcode-testautomation\src\test\resources\css\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90087E6F-D08B-40D8-8BC9-0E3FF7DBA035}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4FD4405-F2E8-42CE-A95C-54C49EA55144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="2" xr2:uid="{7CA6F974-39B2-4E5F-BC2D-5AC16F3752B6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7CA6F974-39B2-4E5F-BC2D-5AC16F3752B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer Self Service-Accept" sheetId="2" r:id="rId1"/>
@@ -231,9 +231,6 @@
     <t>EvaluateFunctionVariables</t>
   </si>
   <si>
-    <t>startDate=TEXT(TODAY(),"yyyy-mm-dd")</t>
-  </si>
-  <si>
     <t>AddifyVariables</t>
   </si>
   <si>
@@ -352,20 +349,6 @@
   <si>
     <t>{
     "status": "QUOTE_RECEIVED",
-    "expirationDate": "2022-11-21T04:59:00.000Z",
-    "insurancePremium": {
-        "amount": 500,
-        "currency": "CHF"
-    },
-    "policyLimit": {
-        "amount": 50000,
-        "currency": "CHF"
-    }
-}</t>
-  </si>
-  <si>
-    <t>{
-    "status": "QUOTE_RECEIVED",
     "expirationDate": "2021-11-21T04:59:00.000Z",
     "insurancePremium": {
         "amount": 500,
@@ -385,6 +368,23 @@
   </si>
   <si>
     <t>id=customers[-1].customerId</t>
+  </si>
+  <si>
+    <t>expiryDate=SUBSTITUTE(TEXT(NOW()+365, "yyyy-mm-dd HH:mm:ss"), " ", "T");startDate=TEXT(TODAY(),"yyyy-mm-dd")</t>
+  </si>
+  <si>
+    <t>{
+    "status": "QUOTE_RECEIVED",
+    "expirationDate": "[expiryDate].000Z",
+    "insurancePremium": {
+        "amount": 500,
+        "currency": "CHF"
+    },
+    "policyLimit": {
+        "amount": 50000,
+        "currency": "CHF"
+    }
+}</t>
   </si>
 </sst>
 </file>
@@ -552,7 +552,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -583,6 +583,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="18" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1532,30 +1533,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B87A57E5-F5BD-4861-8936-9E28488C0E70}">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView topLeftCell="F6" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="J5" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.68359375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.41796875" customWidth="1"/>
-    <col min="3" max="3" width="12.41796875" customWidth="1"/>
-    <col min="4" max="4" width="33.83984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="33.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="81" customWidth="1"/>
-    <col min="6" max="6" width="8.83984375" customWidth="1"/>
-    <col min="7" max="7" width="16.15625" customWidth="1"/>
-    <col min="8" max="8" width="14.83984375" customWidth="1"/>
-    <col min="9" max="9" width="21.15625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="54.578125" customWidth="1"/>
-    <col min="11" max="11" width="58.83984375" customWidth="1"/>
-    <col min="12" max="12" width="25.26171875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="111.83984375" customWidth="1"/>
-    <col min="14" max="14" width="25.41796875" customWidth="1"/>
-    <col min="15" max="15" width="14.83984375" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" customWidth="1"/>
+    <col min="9" max="9" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="54.5703125" customWidth="1"/>
+    <col min="11" max="11" width="58.85546875" customWidth="1"/>
+    <col min="12" max="12" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="111.85546875" customWidth="1"/>
+    <col min="14" max="14" width="50.5703125" customWidth="1"/>
+    <col min="15" max="15" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1599,10 +1600,10 @@
         <v>52</v>
       </c>
       <c r="O1" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>28</v>
       </c>
@@ -1641,7 +1642,7 @@
       <c r="N2" s="9"/>
       <c r="O2" s="9"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>21</v>
       </c>
@@ -1677,12 +1678,12 @@
         <v>20</v>
       </c>
       <c r="M3" s="9"/>
-      <c r="N3" s="9" t="s">
-        <v>53</v>
+      <c r="N3" s="13" t="s">
+        <v>84</v>
       </c>
       <c r="O3" s="9"/>
     </row>
-    <row r="4" spans="1:15" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>22</v>
       </c>
@@ -1717,13 +1718,13 @@
       <c r="L4" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="M4" s="9"/>
+      <c r="M4" s="20"/>
       <c r="N4" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="O4" s="9"/>
     </row>
-    <row r="5" spans="1:15" ht="374.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:15" ht="390" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>32</v>
       </c>
@@ -1752,7 +1753,7 @@
         <v>27</v>
       </c>
       <c r="J5" s="11" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="K5" s="8"/>
       <c r="L5" s="6" t="s">
@@ -1761,10 +1762,10 @@
       <c r="M5" s="9"/>
       <c r="N5" s="9"/>
       <c r="O5" s="9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="172.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:15" ht="180" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>40</v>
       </c>
@@ -1793,7 +1794,7 @@
         <v>27</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>81</v>
+        <v>85</v>
       </c>
       <c r="K6" s="8" t="s">
         <v>34</v>
@@ -1803,7 +1804,7 @@
       <c r="N6" s="9"/>
       <c r="O6" s="9"/>
     </row>
-    <row r="7" spans="1:15" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:15" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>36</v>
       </c>
@@ -1871,24 +1872,24 @@
       <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.68359375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.41796875" customWidth="1"/>
-    <col min="3" max="3" width="12.41796875" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.42578125" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
     <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="80.15625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.83984375" customWidth="1"/>
-    <col min="7" max="7" width="16.15625" customWidth="1"/>
-    <col min="8" max="8" width="14.83984375" customWidth="1"/>
-    <col min="9" max="9" width="21.15625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="54.578125" customWidth="1"/>
+    <col min="5" max="5" width="80.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" customWidth="1"/>
+    <col min="7" max="7" width="16.140625" customWidth="1"/>
+    <col min="8" max="8" width="14.85546875" customWidth="1"/>
+    <col min="9" max="9" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="54.5703125" customWidth="1"/>
     <col min="11" max="11" width="27" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.26171875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="24.578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="24.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1932,7 +1933,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>28</v>
       </c>
@@ -1970,7 +1971,7 @@
       <c r="M2" s="9"/>
       <c r="N2" s="9"/>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>21</v>
       </c>
@@ -2008,7 +2009,7 @@
       <c r="M3" s="9"/>
       <c r="N3" s="9"/>
     </row>
-    <row r="4" spans="1:14" ht="72" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:14" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>22</v>
       </c>
@@ -2046,7 +2047,7 @@
       <c r="M4" s="9"/>
       <c r="N4" s="9"/>
     </row>
-    <row r="5" spans="1:14" ht="374.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:14" ht="390" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>47</v>
       </c>
@@ -2084,7 +2085,7 @@
       <c r="M5" s="9"/>
       <c r="N5" s="9"/>
     </row>
-    <row r="6" spans="1:14" ht="172.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:14" ht="180" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>46</v>
       </c>
@@ -2113,7 +2114,7 @@
         <v>27</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="K6" s="8" t="s">
         <v>45</v>
@@ -2122,7 +2123,7 @@
       <c r="M6" s="9"/>
       <c r="N6" s="9"/>
     </row>
-    <row r="7" spans="1:14" ht="158.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:14" ht="195" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>41</v>
       </c>
@@ -2185,27 +2186,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50E57E3D-0C14-46A6-9520-2A3B86BE3763}">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.15625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5.26171875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="38.41796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="53" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.68359375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.26171875" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="34.47265625" customWidth="1"/>
-    <col min="11" max="11" width="55.41796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="65.41796875" customWidth="1"/>
-    <col min="13" max="13" width="24.9453125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="28.05078125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="34.42578125" customWidth="1"/>
+    <col min="11" max="11" width="55.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="65.42578125" customWidth="1"/>
+    <col min="13" max="13" width="25" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="28" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2234,7 +2235,7 @@
         <v>13</v>
       </c>
       <c r="J1" s="16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="K1" s="4" t="s">
         <v>14</v>
@@ -2249,22 +2250,22 @@
         <v>52</v>
       </c>
       <c r="O1" s="19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:15" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>19</v>
@@ -2279,25 +2280,25 @@
       <c r="J2" s="17"/>
       <c r="K2" s="15"/>
       <c r="L2" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="O2" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>19</v>
@@ -2312,25 +2313,25 @@
       <c r="J3" s="17"/>
       <c r="K3" s="15"/>
       <c r="L3" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C4" s="6"/>
       <c r="D4" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>19</v>
@@ -2345,15 +2346,15 @@
       <c r="J4" s="17"/>
       <c r="K4" s="15"/>
       <c r="L4" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>8</v>
@@ -2362,10 +2363,10 @@
         <v>38</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>19</v>
@@ -2379,18 +2380,18 @@
       <c r="I5" s="17"/>
       <c r="J5" s="17"/>
       <c r="K5" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="L5" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="O5" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>8</v>
@@ -2399,10 +2400,10 @@
         <v>38</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>19</v>
@@ -2418,25 +2419,25 @@
       <c r="K6" s="15"/>
       <c r="L6" s="11"/>
       <c r="M6" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="O6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:15" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>8</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>11</v>
@@ -2448,19 +2449,19 @@
         <v>200</v>
       </c>
       <c r="I7" s="18" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J7" s="18">
         <v>65</v>
       </c>
       <c r="M7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="N7" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="O7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Disabled auto report generation
</commit_message>
<xml_diff>
--- a/src/test/resources/css/customer-self-service.xlsx
+++ b/src/test/resources/css/customer-self-service.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\virtualan-software-delivery\September-release\microservices-lowcode-testautomation\src\test\resources\css\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4FD4405-F2E8-42CE-A95C-54C49EA55144}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{774CEC8F-235C-464D-AD75-6C7924D690EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7CA6F974-39B2-4E5F-BC2D-5AC16F3752B6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{7CA6F974-39B2-4E5F-BC2D-5AC16F3752B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer Self Service-Accept" sheetId="2" r:id="rId1"/>
@@ -1533,7 +1533,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B87A57E5-F5BD-4861-8936-9E28488C0E70}">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J5" workbookViewId="0">
+    <sheetView topLeftCell="F5" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
@@ -2186,8 +2186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{50E57E3D-0C14-46A6-9520-2A3B86BE3763}">
   <dimension ref="A1:O7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Keep track for feature file changes as well
</commit_message>
<xml_diff>
--- a/src/test/resources/css/customer-self-service.xlsx
+++ b/src/test/resources/css/customer-self-service.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\virtualan-software-delivery\September-release\microservices-lowcode-testautomation\src\test\resources\css\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35F510D3-9B75-4976-81A1-445DE556351C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F749B63-1DB4-4829-B734-8A92947A5EF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{7CA6F974-39B2-4E5F-BC2D-5AC16F3752B6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7CA6F974-39B2-4E5F-BC2D-5AC16F3752B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Customer Self Service-Accept" sheetId="2" r:id="rId1"/>
     <sheet name="Customer Self-Service-Reject" sheetId="1" r:id="rId2"/>
     <sheet name="Examples" sheetId="3" r:id="rId3"/>
+    <sheet name="Graphql-Example" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="113">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -378,12 +379,119 @@
   <si>
     <t>http://localhost/auth</t>
   </si>
+  <si>
+    <t>http://localhost:8080/apis/graphql</t>
+  </si>
+  <si>
+    <t>Create-User-using-Graphql</t>
+  </si>
+  <si>
+    <t>graphql</t>
+  </si>
+  <si>
+    <t>Create user with Graphql</t>
+  </si>
+  <si>
+    <t>data.createAuthor.name=[name]</t>
+  </si>
+  <si>
+    <t>id=data.createAuthor.id</t>
+  </si>
+  <si>
+    <t>Create-AnotherUser-using-Graphql</t>
+  </si>
+  <si>
+    <t>Create another user with Graphql</t>
+  </si>
+  <si>
+    <t>IncludesByPath</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>{
+    "data": {
+        "createAuthor": {
+            "id": "1",
+            "[name]": "bezkoder"
+        }
+    }
+}</t>
+  </si>
+  <si>
+    <t>data.createAuthor/name
+[name]</t>
+  </si>
+  <si>
+    <t>name=suki;age=13;</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> @graphql</t>
+  </si>
+  <si>
+    <t>Read user - using graphql</t>
+  </si>
+  <si>
+    <t>{"query":"query findAllAuthors {\n findAllAuthors {\n id\n name\n age\n }\n}","variables":{}}</t>
+  </si>
+  <si>
+    <t>Read-Graphql-user</t>
+  </si>
+  <si>
+    <t>id2=data.createAuthor.id</t>
+  </si>
+  <si>
+    <t>data.createAuthor/name
+[name2]</t>
+  </si>
+  <si>
+    <t>data.createAuthor.name=[name2]</t>
+  </si>
+  <si>
+    <t>jsonpath=data.findAllAuthors
+id,name,age
+[id],[name], i~13
+[id2],[name2], i~8</t>
+  </si>
+  <si>
+    <t>{"query":"mutation {\n createAuthor(\n name: \"[name]\",\n age: [age]) {\n id name\n }\n}","variables":{
+"name": "",
+"age": 0
+}}</t>
+  </si>
+  <si>
+    <t>name2=sri;age2=8;</t>
+  </si>
+  <si>
+    <t>{"query":"mutation {\n createAuthor(\n name: \"[name2]\",\n age: [age2]) {\n id name\n }\n}","variables":{
+"name": "",
+"age": 0
+}}</t>
+  </si>
+  <si>
+    <t>insurancePremiumAmount=500</t>
+  </si>
+  <si>
+    <t>{
+    "status": "QUOTE_RECEIVED",
+    "expirationDate": "[expiryDate].000Z",
+    "insurancePremium": {
+        "amount": "[insurancePremiumAmount]",
+        "currency": "CHF"
+    },
+    "policyLimit": {
+        "amount": 50000,
+        "currency": "CHF"
+    }
+}</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -412,6 +520,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF212121"/>
+      <name val="Courier New"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -544,7 +658,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -576,6 +690,14 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="18" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1542,7 +1664,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B87A57E5-F5BD-4861-8936-9E28488C0E70}">
   <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView topLeftCell="I6" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I6" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
@@ -1697,7 +1819,9 @@
       <c r="N3" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="O3" s="9"/>
+      <c r="O3" s="9" t="s">
+        <v>111</v>
+      </c>
       <c r="P3" s="9"/>
     </row>
     <row r="4" spans="1:16" ht="75" x14ac:dyDescent="0.25">
@@ -1813,7 +1937,7 @@
         <v>27</v>
       </c>
       <c r="J6" s="11" t="s">
-        <v>84</v>
+        <v>112</v>
       </c>
       <c r="K6" s="8" t="s">
         <v>34</v>
@@ -1901,7 +2025,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{558B51E2-E984-41DF-9C0A-F557E24A35FA}">
   <dimension ref="A1:N7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I6" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
@@ -2222,7 +2346,7 @@
   <dimension ref="A1:O7"/>
   <sheetViews>
     <sheetView topLeftCell="J1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q3" sqref="Q3"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2508,4 +2632,227 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAB4DF19-83A5-4FEA-9E34-BA6EFC9624BD}">
+  <dimension ref="A1:Q4"/>
+  <sheetViews>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="43.85546875" customWidth="1"/>
+    <col min="10" max="10" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="45.140625" customWidth="1"/>
+    <col min="12" max="12" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="59.140625" customWidth="1"/>
+    <col min="14" max="14" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="18.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="J1" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" s="23" t="s">
+        <v>95</v>
+      </c>
+      <c r="M1" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="N1" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="O1" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="P1" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="Q1" s="19" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="150" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>88</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2">
+        <v>200</v>
+      </c>
+      <c r="I2" s="22" t="s">
+        <v>108</v>
+      </c>
+      <c r="J2" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="K2" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="L2" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="M2" s="22" t="s">
+        <v>98</v>
+      </c>
+      <c r="N2" s="22" t="s">
+        <v>92</v>
+      </c>
+      <c r="P2" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q2" s="22" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="150" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E3" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="F3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3">
+        <v>200</v>
+      </c>
+      <c r="I3" s="22" t="s">
+        <v>110</v>
+      </c>
+      <c r="J3" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="K3" s="22" t="s">
+        <v>106</v>
+      </c>
+      <c r="L3" s="22" t="s">
+        <v>96</v>
+      </c>
+      <c r="M3" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="N3" s="22" t="s">
+        <v>104</v>
+      </c>
+      <c r="P3" s="22" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="F4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H4">
+        <v>200</v>
+      </c>
+      <c r="I4" s="24" t="s">
+        <v>102</v>
+      </c>
+      <c r="M4" s="22" t="s">
+        <v>107</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{180ACA25-F756-4186-AC24-3FC418FE698B}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{23BC7330-EC62-4BD5-9C0B-B916C1920717}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{64BB8EA6-8648-4E15-8252-996EBFC66AED}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId4"/>
+</worksheet>
 </file>
</xml_diff>